<commit_message>
Updates on specific rates
</commit_message>
<xml_diff>
--- a/Data/ZeLa Data/ELN_Excel data sheet_Bio141 to Bio148.xlsx
+++ b/Data/ZeLa Data/ELN_Excel data sheet_Bio141 to Bio148.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pablodigiusto/Documents/GitHub/Whole-Cell-Network-Reconstruction-for-CHO-cells/Data/ZeLa Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\DC\Manual curation_iCHO\Whole-Cell-Network-Reconstruction-for-CHO-cells_origin\Whole-Cell-Network-Reconstruction-for-CHO-cells\Data\ZeLa Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DFFEFA-FB32-2144-8AF0-E63EE62AFACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15E1F8E-86AC-4E9A-9780-17F8BCFEC3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36640" yWindow="500" windowWidth="34720" windowHeight="18440" tabRatio="888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All data" sheetId="20" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -496,9 +494,6 @@
     <t>Sample Volume</t>
   </si>
   <si>
-    <t>Total Volume</t>
-  </si>
-  <si>
     <t>Accum Sample Volume</t>
   </si>
   <si>
@@ -528,20 +523,24 @@
   <si>
     <t>Adjusted by volume</t>
   </si>
+  <si>
+    <t>Total Volume</t>
+    <phoneticPr fontId="35" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_)"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="hh:mm;@"/>
-    <numFmt numFmtId="168" formatCode="yyyy/mm/dd;@"/>
-    <numFmt numFmtId="169" formatCode="0.00000"/>
+    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="177" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_)"/>
+    <numFmt numFmtId="178" formatCode="0.000"/>
+    <numFmt numFmtId="179" formatCode="hh:mm;@"/>
+    <numFmt numFmtId="180" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="181" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -549,42 +548,42 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -619,7 +618,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Cambria"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -627,7 +626,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -635,7 +634,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -643,35 +642,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -679,7 +678,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -687,14 +686,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -702,14 +701,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -717,7 +716,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -725,20 +724,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -750,7 +749,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -777,6 +776,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="38">
@@ -1336,7 +1341,7 @@
   </borders>
   <cellStyleXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1462,10 +1467,10 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1498,23 +1503,23 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="36" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1540,14 +1545,14 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="178" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="178" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1557,7 +1562,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1573,19 +1578,19 @@
     <xf numFmtId="1" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1597,49 +1602,49 @@
     <xf numFmtId="1" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1648,13 +1653,13 @@
     <xf numFmtId="1" fontId="32" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="36" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1753,7 +1758,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="36" borderId="10" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="178" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1774,7 +1779,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1787,7 +1792,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1797,7 +1802,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="8" fillId="36" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1814,125 +1819,106 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="37" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="75"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="75" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="75" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="89" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="89" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="9" xfId="89" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="89" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="9" xfId="89" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="89" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="36" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="20" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="7" fillId="36" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="7" fillId="36" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="36" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="36" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="7" fillId="36" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="7" fillId="36" borderId="13" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="7" fillId="36" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="0" fillId="36" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="0" fillId="36" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="7" fillId="36" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="103">
-    <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="20% - Accent1 3" xfId="61" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="20% - Accent1 4" xfId="77" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="20% - Accent1 5" xfId="91" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent2 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="20% - Accent2 3" xfId="63" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="20% - Accent2 4" xfId="79" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="20% - Accent2 5" xfId="93" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
     <cellStyle name="20% - Accent3 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="20% - Accent3 3" xfId="65" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="20% - Accent3 4" xfId="81" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="20% - Accent3 5" xfId="95" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="1"/>
     <cellStyle name="20% - Accent4 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="20% - Accent4 3" xfId="67" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="20% - Accent4 4" xfId="83" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
     <cellStyle name="20% - Accent4 5" xfId="97" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="1"/>
     <cellStyle name="20% - Accent5 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
     <cellStyle name="20% - Accent5 3" xfId="69" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
     <cellStyle name="20% - Accent5 4" xfId="85" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
     <cellStyle name="20% - Accent5 5" xfId="99" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="1"/>
     <cellStyle name="20% - Accent6 2" xfId="57" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
     <cellStyle name="20% - Accent6 3" xfId="71" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
     <cellStyle name="20% - Accent6 4" xfId="87" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
     <cellStyle name="20% - Accent6 5" xfId="101" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색1" xfId="20" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색2" xfId="24" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색3" xfId="28" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색4" xfId="32" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색5" xfId="36" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색6" xfId="40" builtinId="50" customBuiltin="1"/>
     <cellStyle name="40% - Accent1 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
     <cellStyle name="40% - Accent1 3" xfId="62" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
     <cellStyle name="40% - Accent1 4" xfId="78" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
     <cellStyle name="40% - Accent1 5" xfId="92" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="1"/>
     <cellStyle name="40% - Accent2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
     <cellStyle name="40% - Accent2 3" xfId="64" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
     <cellStyle name="40% - Accent2 4" xfId="80" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
     <cellStyle name="40% - Accent2 5" xfId="94" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="1"/>
     <cellStyle name="40% - Accent3 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
     <cellStyle name="40% - Accent3 3" xfId="66" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
     <cellStyle name="40% - Accent3 4" xfId="82" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
     <cellStyle name="40% - Accent3 5" xfId="96" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="1"/>
     <cellStyle name="40% - Accent4 2" xfId="54" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
     <cellStyle name="40% - Accent4 3" xfId="68" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
     <cellStyle name="40% - Accent4 4" xfId="84" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
     <cellStyle name="40% - Accent4 5" xfId="98" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Accent5 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
     <cellStyle name="40% - Accent5 3" xfId="70" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
     <cellStyle name="40% - Accent5 4" xfId="86" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
     <cellStyle name="40% - Accent5 5" xfId="100" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="1"/>
     <cellStyle name="40% - Accent6 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
     <cellStyle name="40% - Accent6 3" xfId="72" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
     <cellStyle name="40% - Accent6 4" xfId="88" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
     <cellStyle name="40% - Accent6 5" xfId="102" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="34" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="38" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="42" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="23" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="27" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="9" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="13" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="15" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색1" xfId="21" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색2" xfId="25" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색3" xfId="29" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색4" xfId="33" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색5" xfId="37" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색6" xfId="41" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 강조색1" xfId="22" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 강조색2" xfId="26" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 강조색3" xfId="30" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 강조색4" xfId="34" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 강조색5" xfId="38" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 강조색6" xfId="42" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Euro" xfId="1" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="8" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="4" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="5" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="6" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="7" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="11" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="14" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="10" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
     <cellStyle name="Normal 3" xfId="45" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
     <cellStyle name="Normal 4" xfId="59" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
@@ -1946,10 +1932,29 @@
     <cellStyle name="Note 4" xfId="60" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
     <cellStyle name="Note 5" xfId="76" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
     <cellStyle name="Note 6" xfId="90" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="Output" xfId="12" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="3" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="16" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="강조색1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="강조색2" xfId="23" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="강조색3" xfId="27" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="강조색4" xfId="31" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="강조색5" xfId="35" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="강조색6" xfId="39" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="경고문" xfId="16" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="계산" xfId="13" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="나쁨" xfId="9" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="보통" xfId="10" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="설명 텍스트" xfId="17" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="셀 확인" xfId="15" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="연결된 셀" xfId="14" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="요약" xfId="18" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="입력" xfId="11" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="제목" xfId="3" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="제목 1" xfId="4" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="제목 2" xfId="5" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="제목 3" xfId="6" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="제목 4" xfId="7" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="좋음" xfId="8" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="출력" xfId="12" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2040,7 +2045,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3527,7 +3532,7 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-AR"/>
+            <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
       </c:legendEntry>
@@ -3549,7 +3554,7 @@
           <a:pPr>
             <a:defRPr sz="1200" b="1"/>
           </a:pPr>
-          <a:endParaRPr lang="en-AR"/>
+          <a:endParaRPr lang="ko-KR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3564,7 +3569,7 @@
       <a:pPr>
         <a:defRPr sz="1100"/>
       </a:pPr>
-      <a:endParaRPr lang="en-AR"/>
+      <a:endParaRPr lang="ko-KR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3579,7 +3584,7 @@
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5091,7 +5096,7 @@
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6640,7 +6645,7 @@
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -8187,7 +8192,7 @@
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -8550,37 +8555,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.4</c:v>
+                  <c:v>9.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.600000000000001</c:v>
+                  <c:v>14.100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16.100000000000001</c:v>
+                  <c:v>18.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.6</c:v>
+                  <c:v>23.1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23.6</c:v>
+                  <c:v>26.1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25.8</c:v>
+                  <c:v>28.3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>27.5</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>29</c:v>
+                  <c:v>31.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>30</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9688,7 +9693,7 @@
 <file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -11189,7 +11194,7 @@
 <file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -12738,7 +12743,7 @@
 <file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -14608,7 +14613,7 @@
           <a:pPr rtl="0">
             <a:defRPr/>
           </a:pPr>
-          <a:endParaRPr lang="en-AR"/>
+          <a:endParaRPr lang="ko-KR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -14641,7 +14646,7 @@
 <file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -16550,7 +16555,7 @@
           <a:pPr rtl="0">
             <a:defRPr/>
           </a:pPr>
-          <a:endParaRPr lang="en-AR"/>
+          <a:endParaRPr lang="ko-KR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -16583,7 +16588,7 @@
 <file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -18067,7 +18072,7 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-AR"/>
+            <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
       </c:legendEntry>
@@ -18089,7 +18094,7 @@
           <a:pPr>
             <a:defRPr sz="1000"/>
           </a:pPr>
-          <a:endParaRPr lang="en-AR"/>
+          <a:endParaRPr lang="ko-KR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -18122,7 +18127,7 @@
 <file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -19420,7 +19425,7 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-AR"/>
+            <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
       </c:legendEntry>
@@ -19442,7 +19447,7 @@
           <a:pPr>
             <a:defRPr sz="1000"/>
           </a:pPr>
-          <a:endParaRPr lang="en-AR"/>
+          <a:endParaRPr lang="ko-KR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -19475,7 +19480,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -20959,7 +20964,7 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-AR"/>
+            <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
       </c:legendEntry>
@@ -20981,7 +20986,7 @@
           <a:pPr>
             <a:defRPr sz="1000"/>
           </a:pPr>
-          <a:endParaRPr lang="en-AR"/>
+          <a:endParaRPr lang="ko-KR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -21014,7 +21019,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -22515,7 +22520,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -24062,7 +24067,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -25608,7 +25613,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -27155,7 +27160,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -28704,7 +28709,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -29977,7 +29982,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -33825,7 +33830,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="All the data"/>
@@ -34811,49 +34816,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AH243"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="AE30" sqref="AE30"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" customWidth="1"/>
-    <col min="9" max="9" width="9.5" customWidth="1"/>
-    <col min="10" max="12" width="8.33203125" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="12" width="8.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
     <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.33203125" customWidth="1"/>
-    <col min="23" max="23" width="17.1640625" customWidth="1"/>
-    <col min="24" max="24" width="22.83203125" customWidth="1"/>
-    <col min="25" max="25" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.83203125" customWidth="1"/>
-    <col min="32" max="32" width="14.6640625" customWidth="1"/>
-    <col min="33" max="33" width="13.1640625" style="167" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.28515625" customWidth="1"/>
+    <col min="23" max="23" width="17.140625" customWidth="1"/>
+    <col min="24" max="24" width="22.85546875" customWidth="1"/>
+    <col min="25" max="25" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.85546875" customWidth="1"/>
+    <col min="32" max="32" width="14.7109375" customWidth="1"/>
+    <col min="33" max="33" width="13.140625" style="167" customWidth="1"/>
     <col min="34" max="34" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G2" s="7"/>
       <c r="H2" s="9"/>
     </row>
-    <row r="3" spans="1:15" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G3" s="7"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:15" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D4" s="92" t="s">
         <v>76</v>
       </c>
@@ -34885,7 +34890,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D5" s="137" t="s">
         <v>75</v>
       </c>
@@ -34917,7 +34922,7 @@
         <v>0.17299999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -34958,7 +34963,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -34999,7 +35004,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -35040,7 +35045,7 @@
         <v>32.4</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -35077,7 +35082,7 @@
       <c r="N9" s="141"/>
       <c r="O9" s="135"/>
     </row>
-    <row r="10" spans="1:15" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -35118,7 +35123,7 @@
         <v>1.99</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>82</v>
       </c>
@@ -35159,7 +35164,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -35200,7 +35205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -35241,14 +35246,14 @@
         <v>2220</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C14" s="30"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C15" s="30"/>
     </row>
-    <row r="16" spans="1:15" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="1:34" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:34" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="95" t="s">
         <v>44</v>
       </c>
@@ -35314,7 +35319,7 @@
       <c r="AG17" s="174"/>
       <c r="AH17" s="175"/>
     </row>
-    <row r="18" spans="1:34" ht="29" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="103" t="s">
         <v>91</v>
       </c>
@@ -35349,7 +35354,7 @@
         <v>87</v>
       </c>
       <c r="L18" s="164" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M18" s="114" t="s">
         <v>85</v>
@@ -35382,34 +35387,34 @@
         <v>94</v>
       </c>
       <c r="W18" s="112" t="s">
+        <v>105</v>
+      </c>
+      <c r="X18" s="113" t="s">
         <v>95</v>
       </c>
-      <c r="X18" s="113" t="s">
+      <c r="Y18" s="105" t="s">
         <v>96</v>
       </c>
-      <c r="Y18" s="105" t="s">
+      <c r="Z18" s="115" t="s">
         <v>97</v>
       </c>
-      <c r="Z18" s="115" t="s">
+      <c r="AA18" s="116" t="s">
         <v>98</v>
       </c>
-      <c r="AA18" s="116" t="s">
+      <c r="AB18" s="116" t="s">
         <v>99</v>
       </c>
-      <c r="AB18" s="116" t="s">
+      <c r="AC18" s="112" t="s">
         <v>100</v>
       </c>
-      <c r="AC18" s="112" t="s">
+      <c r="AD18" s="112" t="s">
         <v>101</v>
-      </c>
-      <c r="AD18" s="112" t="s">
-        <v>102</v>
       </c>
       <c r="AE18" s="117"/>
       <c r="AF18" s="118"/>
       <c r="AG18" s="172"/>
       <c r="AH18" s="176" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:34" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -35506,13 +35511,13 @@
         <v>43</v>
       </c>
       <c r="AG19" s="173" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH19" s="171" t="s">
         <v>104</v>
       </c>
-      <c r="AH19" s="171" t="s">
-        <v>105</v>
-      </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>59</v>
       </c>
@@ -35581,7 +35586,7 @@
       <c r="AG20" s="168"/>
       <c r="AH20" s="169"/>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>59</v>
       </c>
@@ -35683,7 +35688,7 @@
       <c r="AG21" s="169"/>
       <c r="AH21" s="169"/>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>59</v>
       </c>
@@ -35792,7 +35797,7 @@
       </c>
       <c r="AH22" s="169"/>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>59</v>
       </c>
@@ -35901,7 +35906,7 @@
       </c>
       <c r="AH23" s="169"/>
     </row>
-    <row r="24" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>59</v>
       </c>
@@ -36012,7 +36017,7 @@
       </c>
       <c r="AH24" s="169"/>
     </row>
-    <row r="25" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>59</v>
       </c>
@@ -36092,7 +36097,8 @@
         <v>2.5</v>
       </c>
       <c r="Z25" s="33">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.5</v>
       </c>
       <c r="AA25" s="33">
         <v>8</v>
@@ -36122,7 +36128,7 @@
       </c>
       <c r="AH25" s="169"/>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>59</v>
       </c>
@@ -36203,7 +36209,7 @@
       </c>
       <c r="Z26" s="33">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="AA26" s="33">
         <v>12.6</v>
@@ -36233,7 +36239,7 @@
       </c>
       <c r="AH26" s="169"/>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
         <v>59</v>
       </c>
@@ -36314,7 +36320,7 @@
       </c>
       <c r="Z27" s="33">
         <f t="shared" si="0"/>
-        <v>7.4</v>
+        <v>9.9</v>
       </c>
       <c r="AA27" s="33">
         <v>15.4</v>
@@ -36339,12 +36345,12 @@
         <v>68.731359974376019</v>
       </c>
       <c r="AG27" s="169">
-        <f t="shared" ref="AG27:AH90" si="9">LN(2)/AF27</f>
+        <f t="shared" ref="AG27:AG90" si="9">LN(2)/AF27</f>
         <v>1.0084875096584149E-2</v>
       </c>
       <c r="AH27" s="169"/>
     </row>
-    <row r="28" spans="1:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>59</v>
       </c>
@@ -36428,7 +36434,7 @@
       </c>
       <c r="Z28" s="33">
         <f t="shared" si="0"/>
-        <v>11.600000000000001</v>
+        <v>14.100000000000001</v>
       </c>
       <c r="AA28" s="33">
         <v>0</v>
@@ -36458,7 +36464,7 @@
       </c>
       <c r="AH28" s="169"/>
     </row>
-    <row r="29" spans="1:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>59</v>
       </c>
@@ -36542,7 +36548,7 @@
       </c>
       <c r="Z29" s="33">
         <f t="shared" si="0"/>
-        <v>16.100000000000001</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="AA29" s="33">
         <v>0</v>
@@ -36572,7 +36578,7 @@
       </c>
       <c r="AH29" s="169"/>
     </row>
-    <row r="30" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>59</v>
       </c>
@@ -36656,7 +36662,7 @@
       </c>
       <c r="Z30" s="33">
         <f t="shared" si="0"/>
-        <v>20.6</v>
+        <v>23.1</v>
       </c>
       <c r="AA30" s="33">
         <v>0</v>
@@ -36686,7 +36692,7 @@
       </c>
       <c r="AH30" s="169"/>
     </row>
-    <row r="31" spans="1:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
         <v>59</v>
       </c>
@@ -36770,7 +36776,7 @@
       </c>
       <c r="Z31" s="33">
         <f t="shared" si="0"/>
-        <v>23.6</v>
+        <v>26.1</v>
       </c>
       <c r="AA31" s="33">
         <v>0</v>
@@ -36800,7 +36806,7 @@
       </c>
       <c r="AH31" s="169"/>
     </row>
-    <row r="32" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
         <v>59</v>
       </c>
@@ -36884,7 +36890,7 @@
       </c>
       <c r="Z32" s="33">
         <f t="shared" si="0"/>
-        <v>25.8</v>
+        <v>28.3</v>
       </c>
       <c r="AA32" s="33">
         <v>0</v>
@@ -36914,7 +36920,7 @@
       </c>
       <c r="AH32" s="169"/>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>59</v>
       </c>
@@ -36996,7 +37002,7 @@
       </c>
       <c r="Z33" s="33">
         <f t="shared" si="0"/>
-        <v>27.5</v>
+        <v>30</v>
       </c>
       <c r="AA33" s="33">
         <v>0</v>
@@ -37026,7 +37032,7 @@
       </c>
       <c r="AH33" s="169"/>
     </row>
-    <row r="34" spans="1:34" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
         <v>59</v>
       </c>
@@ -37108,7 +37114,7 @@
       </c>
       <c r="Z34" s="33">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>31.5</v>
       </c>
       <c r="AA34" s="33">
         <v>0</v>
@@ -37138,7 +37144,7 @@
       </c>
       <c r="AH34" s="169"/>
     </row>
-    <row r="35" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:34" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
         <v>59</v>
       </c>
@@ -37220,7 +37226,7 @@
       </c>
       <c r="Z35" s="70">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>32.5</v>
       </c>
       <c r="AA35" s="69">
         <v>0</v>
@@ -37241,7 +37247,7 @@
       <c r="AG35" s="170"/>
       <c r="AH35" s="170"/>
     </row>
-    <row r="36" spans="1:34" ht="14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:34" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>60</v>
       </c>
@@ -37310,7 +37316,7 @@
       <c r="AG36" s="168"/>
       <c r="AH36" s="168"/>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
         <v>60</v>
       </c>
@@ -37412,7 +37418,7 @@
       <c r="AG37" s="169"/>
       <c r="AH37" s="169"/>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>60</v>
       </c>
@@ -37523,7 +37529,7 @@
       </c>
       <c r="AH38" s="169"/>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
         <v>60</v>
       </c>
@@ -37634,7 +37640,7 @@
       </c>
       <c r="AH39" s="169"/>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
         <v>60</v>
       </c>
@@ -37745,7 +37751,7 @@
       </c>
       <c r="AH40" s="169"/>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
         <v>60</v>
       </c>
@@ -37856,7 +37862,7 @@
       </c>
       <c r="AH41" s="169"/>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
         <v>60</v>
       </c>
@@ -37967,7 +37973,7 @@
       </c>
       <c r="AH42" s="169"/>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
         <v>60</v>
       </c>
@@ -38078,7 +38084,7 @@
       </c>
       <c r="AH43" s="169"/>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
         <v>60</v>
       </c>
@@ -38192,7 +38198,7 @@
       </c>
       <c r="AH44" s="169"/>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
         <v>60</v>
       </c>
@@ -38306,7 +38312,7 @@
       </c>
       <c r="AH45" s="169"/>
     </row>
-    <row r="46" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
         <v>60</v>
       </c>
@@ -38420,7 +38426,7 @@
       </c>
       <c r="AH46" s="169"/>
     </row>
-    <row r="47" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
         <v>60</v>
       </c>
@@ -38534,7 +38540,7 @@
       </c>
       <c r="AH47" s="169"/>
     </row>
-    <row r="48" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
         <v>60</v>
       </c>
@@ -38648,7 +38654,7 @@
       </c>
       <c r="AH48" s="169"/>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
         <v>60</v>
       </c>
@@ -38760,7 +38766,7 @@
       </c>
       <c r="AH49" s="169"/>
     </row>
-    <row r="50" spans="1:34" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A50" s="17" t="s">
         <v>60</v>
       </c>
@@ -38872,7 +38878,7 @@
       </c>
       <c r="AH50" s="169"/>
     </row>
-    <row r="51" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:34" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="23" t="s">
         <v>60</v>
       </c>
@@ -38975,7 +38981,7 @@
       <c r="AG51" s="170"/>
       <c r="AH51" s="170"/>
     </row>
-    <row r="52" spans="1:34" ht="14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:34" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
         <v>61</v>
       </c>
@@ -39044,7 +39050,7 @@
       <c r="AG52" s="168"/>
       <c r="AH52" s="168"/>
     </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
         <v>61</v>
       </c>
@@ -39146,7 +39152,7 @@
       <c r="AG53" s="169"/>
       <c r="AH53" s="169"/>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A54" s="17" t="s">
         <v>61</v>
       </c>
@@ -39257,7 +39263,7 @@
       </c>
       <c r="AH54" s="169"/>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
         <v>61</v>
       </c>
@@ -39368,7 +39374,7 @@
       </c>
       <c r="AH55" s="169"/>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A56" s="17" t="s">
         <v>61</v>
       </c>
@@ -39479,7 +39485,7 @@
       </c>
       <c r="AH56" s="169"/>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A57" s="17" t="s">
         <v>61</v>
       </c>
@@ -39590,7 +39596,7 @@
       </c>
       <c r="AH57" s="169"/>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A58" s="17" t="s">
         <v>61</v>
       </c>
@@ -39701,7 +39707,7 @@
       </c>
       <c r="AH58" s="169"/>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A59" s="17" t="s">
         <v>61</v>
       </c>
@@ -39812,7 +39818,7 @@
       </c>
       <c r="AH59" s="169"/>
     </row>
-    <row r="60" spans="1:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="17" t="s">
         <v>61</v>
       </c>
@@ -39926,7 +39932,7 @@
       </c>
       <c r="AH60" s="169"/>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A61" s="17" t="s">
         <v>61</v>
       </c>
@@ -40040,7 +40046,7 @@
       </c>
       <c r="AH61" s="169"/>
     </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A62" s="17" t="s">
         <v>61</v>
       </c>
@@ -40154,7 +40160,7 @@
       </c>
       <c r="AH62" s="169"/>
     </row>
-    <row r="63" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="17" t="s">
         <v>61</v>
       </c>
@@ -40268,7 +40274,7 @@
       </c>
       <c r="AH63" s="169"/>
     </row>
-    <row r="64" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="17" t="s">
         <v>61</v>
       </c>
@@ -40382,7 +40388,7 @@
       </c>
       <c r="AH64" s="169"/>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A65" s="17" t="s">
         <v>61</v>
       </c>
@@ -40496,7 +40502,7 @@
       </c>
       <c r="AH65" s="169"/>
     </row>
-    <row r="66" spans="1:34" ht="15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A66" s="17" t="s">
         <v>61</v>
       </c>
@@ -40610,7 +40616,7 @@
       </c>
       <c r="AH66" s="169"/>
     </row>
-    <row r="67" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:34" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="23" t="s">
         <v>61</v>
       </c>
@@ -40715,7 +40721,7 @@
       <c r="AG67" s="170"/>
       <c r="AH67" s="170"/>
     </row>
-    <row r="68" spans="1:34" ht="14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:34" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
         <v>62</v>
       </c>
@@ -40785,7 +40791,7 @@
       <c r="AG68" s="168"/>
       <c r="AH68" s="168"/>
     </row>
-    <row r="69" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A69" s="17" t="s">
         <v>62</v>
       </c>
@@ -40887,7 +40893,7 @@
       <c r="AG69" s="169"/>
       <c r="AH69" s="169"/>
     </row>
-    <row r="70" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A70" s="17" t="s">
         <v>62</v>
       </c>
@@ -40996,7 +41002,7 @@
       </c>
       <c r="AH70" s="169"/>
     </row>
-    <row r="71" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A71" s="17" t="s">
         <v>62</v>
       </c>
@@ -41105,7 +41111,7 @@
       </c>
       <c r="AH71" s="169"/>
     </row>
-    <row r="72" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A72" s="17" t="s">
         <v>62</v>
       </c>
@@ -41214,7 +41220,7 @@
       </c>
       <c r="AH72" s="169"/>
     </row>
-    <row r="73" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A73" s="17" t="s">
         <v>62</v>
       </c>
@@ -41325,7 +41331,7 @@
       </c>
       <c r="AH73" s="169"/>
     </row>
-    <row r="74" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A74" s="17" t="s">
         <v>62</v>
       </c>
@@ -41434,7 +41440,7 @@
       </c>
       <c r="AH74" s="169"/>
     </row>
-    <row r="75" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A75" s="17" t="s">
         <v>62</v>
       </c>
@@ -41543,7 +41549,7 @@
       </c>
       <c r="AH75" s="169"/>
     </row>
-    <row r="76" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A76" s="17" t="s">
         <v>62</v>
       </c>
@@ -41652,7 +41658,7 @@
       </c>
       <c r="AH76" s="169"/>
     </row>
-    <row r="77" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A77" s="17" t="s">
         <v>62</v>
       </c>
@@ -41766,7 +41772,7 @@
       </c>
       <c r="AH77" s="169"/>
     </row>
-    <row r="78" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A78" s="17" t="s">
         <v>62</v>
       </c>
@@ -41878,7 +41884,7 @@
       </c>
       <c r="AH78" s="169"/>
     </row>
-    <row r="79" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="17" t="s">
         <v>62</v>
       </c>
@@ -41990,7 +41996,7 @@
       </c>
       <c r="AH79" s="169"/>
     </row>
-    <row r="80" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="17" t="s">
         <v>62</v>
       </c>
@@ -42102,7 +42108,7 @@
       </c>
       <c r="AH80" s="169"/>
     </row>
-    <row r="81" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A81" s="17" t="s">
         <v>62</v>
       </c>
@@ -42214,7 +42220,7 @@
       </c>
       <c r="AH81" s="169"/>
     </row>
-    <row r="82" spans="1:34" ht="15" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A82" s="17" t="s">
         <v>62</v>
       </c>
@@ -42326,7 +42332,7 @@
       </c>
       <c r="AH82" s="169"/>
     </row>
-    <row r="83" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:34" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="23" t="s">
         <v>62</v>
       </c>
@@ -42427,7 +42433,7 @@
       <c r="AG83" s="170"/>
       <c r="AH83" s="170"/>
     </row>
-    <row r="84" spans="1:34" ht="14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:34" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A84" s="17" t="s">
         <v>63</v>
       </c>
@@ -42497,7 +42503,7 @@
       <c r="AG84" s="168"/>
       <c r="AH84" s="168"/>
     </row>
-    <row r="85" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A85" s="17" t="s">
         <v>63</v>
       </c>
@@ -42599,7 +42605,7 @@
       <c r="AG85" s="169"/>
       <c r="AH85" s="169"/>
     </row>
-    <row r="86" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A86" s="17" t="s">
         <v>63</v>
       </c>
@@ -42708,7 +42714,7 @@
       </c>
       <c r="AH86" s="169"/>
     </row>
-    <row r="87" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A87" s="17" t="s">
         <v>63</v>
       </c>
@@ -42817,7 +42823,7 @@
       </c>
       <c r="AH87" s="169"/>
     </row>
-    <row r="88" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A88" s="17" t="s">
         <v>63</v>
       </c>
@@ -42926,7 +42932,7 @@
       </c>
       <c r="AH88" s="169"/>
     </row>
-    <row r="89" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A89" s="17" t="s">
         <v>63</v>
       </c>
@@ -43035,7 +43041,7 @@
       </c>
       <c r="AH89" s="169"/>
     </row>
-    <row r="90" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A90" s="17" t="s">
         <v>63</v>
       </c>
@@ -43144,7 +43150,7 @@
       </c>
       <c r="AH90" s="169"/>
     </row>
-    <row r="91" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A91" s="17" t="s">
         <v>63</v>
       </c>
@@ -43248,12 +43254,12 @@
         <v>42.545254779967365</v>
       </c>
       <c r="AG91" s="169">
-        <f t="shared" ref="AG91:AH147" si="54">LN(2)/AF91</f>
+        <f t="shared" ref="AG91:AG147" si="54">LN(2)/AF91</f>
         <v>1.6291997407107243E-2</v>
       </c>
       <c r="AH91" s="169"/>
     </row>
-    <row r="92" spans="1:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="17" t="s">
         <v>63</v>
       </c>
@@ -43362,7 +43368,7 @@
       </c>
       <c r="AH92" s="169"/>
     </row>
-    <row r="93" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="17" t="s">
         <v>63</v>
       </c>
@@ -43474,7 +43480,7 @@
       </c>
       <c r="AH93" s="169"/>
     </row>
-    <row r="94" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="17" t="s">
         <v>63</v>
       </c>
@@ -43586,7 +43592,7 @@
       </c>
       <c r="AH94" s="169"/>
     </row>
-    <row r="95" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A95" s="17" t="s">
         <v>63</v>
       </c>
@@ -43698,7 +43704,7 @@
       </c>
       <c r="AH95" s="169"/>
     </row>
-    <row r="96" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="17" t="s">
         <v>63</v>
       </c>
@@ -43810,7 +43816,7 @@
       </c>
       <c r="AH96" s="169"/>
     </row>
-    <row r="97" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A97" s="17" t="s">
         <v>63</v>
       </c>
@@ -43922,7 +43928,7 @@
       </c>
       <c r="AH97" s="169"/>
     </row>
-    <row r="98" spans="1:34" ht="15" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A98" s="17" t="s">
         <v>63</v>
       </c>
@@ -44034,7 +44040,7 @@
       </c>
       <c r="AH98" s="169"/>
     </row>
-    <row r="99" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:34" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="23" t="s">
         <v>63</v>
       </c>
@@ -44137,7 +44143,7 @@
       <c r="AG99" s="170"/>
       <c r="AH99" s="170"/>
     </row>
-    <row r="100" spans="1:34" ht="14" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:34" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A100" s="19" t="s">
         <v>64</v>
       </c>
@@ -44207,7 +44213,7 @@
       <c r="AG100" s="168"/>
       <c r="AH100" s="168"/>
     </row>
-    <row r="101" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A101" s="19" t="s">
         <v>64</v>
       </c>
@@ -44309,7 +44315,7 @@
       <c r="AG101" s="169"/>
       <c r="AH101" s="169"/>
     </row>
-    <row r="102" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A102" s="19" t="s">
         <v>64</v>
       </c>
@@ -44418,7 +44424,7 @@
       </c>
       <c r="AH102" s="169"/>
     </row>
-    <row r="103" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A103" s="19" t="s">
         <v>64</v>
       </c>
@@ -44527,7 +44533,7 @@
       </c>
       <c r="AH103" s="169"/>
     </row>
-    <row r="104" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A104" s="19" t="s">
         <v>64</v>
       </c>
@@ -44636,7 +44642,7 @@
       </c>
       <c r="AH104" s="169"/>
     </row>
-    <row r="105" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A105" s="19" t="s">
         <v>64</v>
       </c>
@@ -44745,7 +44751,7 @@
       </c>
       <c r="AH105" s="169"/>
     </row>
-    <row r="106" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A106" s="19" t="s">
         <v>64</v>
       </c>
@@ -44854,7 +44860,7 @@
       </c>
       <c r="AH106" s="169"/>
     </row>
-    <row r="107" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A107" s="19" t="s">
         <v>64</v>
       </c>
@@ -44963,7 +44969,7 @@
       </c>
       <c r="AH107" s="169"/>
     </row>
-    <row r="108" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A108" s="19" t="s">
         <v>64</v>
       </c>
@@ -45072,7 +45078,7 @@
       </c>
       <c r="AH108" s="169"/>
     </row>
-    <row r="109" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A109" s="19" t="s">
         <v>64</v>
       </c>
@@ -45181,7 +45187,7 @@
       </c>
       <c r="AH109" s="169"/>
     </row>
-    <row r="110" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A110" s="19" t="s">
         <v>64</v>
       </c>
@@ -45293,7 +45299,7 @@
       </c>
       <c r="AH110" s="169"/>
     </row>
-    <row r="111" spans="1:34" ht="14.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:34" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="19" t="s">
         <v>64</v>
       </c>
@@ -45405,7 +45411,7 @@
       </c>
       <c r="AH111" s="169"/>
     </row>
-    <row r="112" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A112" s="19" t="s">
         <v>64</v>
       </c>
@@ -45517,7 +45523,7 @@
       </c>
       <c r="AH112" s="169"/>
     </row>
-    <row r="113" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A113" s="19" t="s">
         <v>64</v>
       </c>
@@ -45629,7 +45635,7 @@
       </c>
       <c r="AH113" s="169"/>
     </row>
-    <row r="114" spans="1:34" ht="15" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A114" s="19" t="s">
         <v>64</v>
       </c>
@@ -45741,7 +45747,7 @@
       </c>
       <c r="AH114" s="169"/>
     </row>
-    <row r="115" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:34" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="56" t="s">
         <v>64</v>
       </c>
@@ -45844,7 +45850,7 @@
       <c r="AG115" s="170"/>
       <c r="AH115" s="170"/>
     </row>
-    <row r="116" spans="1:34" ht="14" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:34" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A116" s="19" t="s">
         <v>65</v>
       </c>
@@ -45915,7 +45921,7 @@
       <c r="AG116" s="168"/>
       <c r="AH116" s="168"/>
     </row>
-    <row r="117" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A117" s="19" t="s">
         <v>65</v>
       </c>
@@ -46017,7 +46023,7 @@
       <c r="AG117" s="169"/>
       <c r="AH117" s="169"/>
     </row>
-    <row r="118" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A118" s="19" t="s">
         <v>65</v>
       </c>
@@ -46126,7 +46132,7 @@
       </c>
       <c r="AH118" s="169"/>
     </row>
-    <row r="119" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A119" s="19" t="s">
         <v>65</v>
       </c>
@@ -46235,7 +46241,7 @@
       </c>
       <c r="AH119" s="169"/>
     </row>
-    <row r="120" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A120" s="19" t="s">
         <v>65</v>
       </c>
@@ -46344,7 +46350,7 @@
       </c>
       <c r="AH120" s="169"/>
     </row>
-    <row r="121" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A121" s="19" t="s">
         <v>65</v>
       </c>
@@ -46453,7 +46459,7 @@
       </c>
       <c r="AH121" s="169"/>
     </row>
-    <row r="122" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A122" s="19" t="s">
         <v>65</v>
       </c>
@@ -46562,7 +46568,7 @@
       </c>
       <c r="AH122" s="169"/>
     </row>
-    <row r="123" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A123" s="30" t="s">
         <v>65</v>
       </c>
@@ -46671,7 +46677,7 @@
       </c>
       <c r="AH123" s="169"/>
     </row>
-    <row r="124" spans="1:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="30" t="s">
         <v>65</v>
       </c>
@@ -46780,7 +46786,7 @@
       </c>
       <c r="AH124" s="169"/>
     </row>
-    <row r="125" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A125" s="30" t="s">
         <v>65</v>
       </c>
@@ -46892,7 +46898,7 @@
       </c>
       <c r="AH125" s="169"/>
     </row>
-    <row r="126" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A126" s="30" t="s">
         <v>65</v>
       </c>
@@ -47004,7 +47010,7 @@
       </c>
       <c r="AH126" s="169"/>
     </row>
-    <row r="127" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A127" s="30" t="s">
         <v>65</v>
       </c>
@@ -47116,7 +47122,7 @@
       </c>
       <c r="AH127" s="169"/>
     </row>
-    <row r="128" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A128" s="30" t="s">
         <v>65</v>
       </c>
@@ -47228,7 +47234,7 @@
       </c>
       <c r="AH128" s="169"/>
     </row>
-    <row r="129" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A129" s="30" t="s">
         <v>65</v>
       </c>
@@ -47340,7 +47346,7 @@
       </c>
       <c r="AH129" s="169"/>
     </row>
-    <row r="130" spans="1:34" ht="15" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A130" s="30" t="s">
         <v>65</v>
       </c>
@@ -47452,7 +47458,7 @@
       </c>
       <c r="AH130" s="169"/>
     </row>
-    <row r="131" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:34" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="51" t="s">
         <v>65</v>
       </c>
@@ -47555,7 +47561,7 @@
       <c r="AG131" s="170"/>
       <c r="AH131" s="170"/>
     </row>
-    <row r="132" spans="1:34" ht="14" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:34" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A132" s="17" t="s">
         <v>66</v>
       </c>
@@ -47626,7 +47632,7 @@
       <c r="AG132" s="168"/>
       <c r="AH132" s="168"/>
     </row>
-    <row r="133" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A133" s="17" t="s">
         <v>66</v>
       </c>
@@ -47728,7 +47734,7 @@
       <c r="AG133" s="169"/>
       <c r="AH133" s="169"/>
     </row>
-    <row r="134" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A134" s="17" t="s">
         <v>66</v>
       </c>
@@ -47837,7 +47843,7 @@
       </c>
       <c r="AH134" s="169"/>
     </row>
-    <row r="135" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A135" s="42" t="s">
         <v>66</v>
       </c>
@@ -47946,7 +47952,7 @@
       </c>
       <c r="AH135" s="169"/>
     </row>
-    <row r="136" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A136" s="42" t="s">
         <v>66</v>
       </c>
@@ -48055,7 +48061,7 @@
       </c>
       <c r="AH136" s="169"/>
     </row>
-    <row r="137" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A137" s="42" t="s">
         <v>66</v>
       </c>
@@ -48164,7 +48170,7 @@
       </c>
       <c r="AH137" s="169"/>
     </row>
-    <row r="138" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A138" s="42" t="s">
         <v>66</v>
       </c>
@@ -48273,7 +48279,7 @@
       </c>
       <c r="AH138" s="169"/>
     </row>
-    <row r="139" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A139" s="42" t="s">
         <v>66</v>
       </c>
@@ -48382,7 +48388,7 @@
       </c>
       <c r="AH139" s="169"/>
     </row>
-    <row r="140" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A140" s="42" t="s">
         <v>66</v>
       </c>
@@ -48491,7 +48497,7 @@
       </c>
       <c r="AH140" s="169"/>
     </row>
-    <row r="141" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A141" s="42" t="s">
         <v>66</v>
       </c>
@@ -48603,7 +48609,7 @@
       </c>
       <c r="AH141" s="169"/>
     </row>
-    <row r="142" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A142" s="42" t="s">
         <v>66</v>
       </c>
@@ -48715,7 +48721,7 @@
       </c>
       <c r="AH142" s="169"/>
     </row>
-    <row r="143" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="42" t="s">
         <v>66</v>
       </c>
@@ -48827,7 +48833,7 @@
       </c>
       <c r="AH143" s="169"/>
     </row>
-    <row r="144" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A144" s="42" t="s">
         <v>66</v>
       </c>
@@ -48939,7 +48945,7 @@
       </c>
       <c r="AH144" s="169"/>
     </row>
-    <row r="145" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A145" s="42" t="s">
         <v>66</v>
       </c>
@@ -49051,7 +49057,7 @@
       </c>
       <c r="AH145" s="169"/>
     </row>
-    <row r="146" spans="1:34" ht="15" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:34" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A146" s="17" t="s">
         <v>66</v>
       </c>
@@ -49163,7 +49169,7 @@
       </c>
       <c r="AH146" s="169"/>
     </row>
-    <row r="147" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:34" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A147" s="23" t="s">
         <v>66</v>
       </c>
@@ -49275,7 +49281,7 @@
       </c>
       <c r="AH147" s="170"/>
     </row>
-    <row r="148" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C148" s="1"/>
       <c r="D148" s="2"/>
       <c r="E148" s="2"/>
@@ -49307,7 +49313,7 @@
       <c r="AE148" s="3"/>
       <c r="AF148" s="3"/>
     </row>
-    <row r="149" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C149" s="1"/>
       <c r="D149" s="2"/>
       <c r="E149" s="2"/>
@@ -49339,7 +49345,7 @@
       <c r="AE149" s="3"/>
       <c r="AF149" s="3"/>
     </row>
-    <row r="150" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C150" s="1"/>
       <c r="D150" s="2"/>
       <c r="E150" s="2"/>
@@ -49371,7 +49377,7 @@
       <c r="AE150" s="3"/>
       <c r="AF150" s="3"/>
     </row>
-    <row r="151" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C151" s="1"/>
       <c r="D151" s="2"/>
       <c r="E151" s="2"/>
@@ -49403,7 +49409,7 @@
       <c r="AE151" s="3"/>
       <c r="AF151" s="3"/>
     </row>
-    <row r="152" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C152" s="1"/>
       <c r="D152" s="2"/>
       <c r="E152" s="2"/>
@@ -49435,7 +49441,7 @@
       <c r="AE152" s="3"/>
       <c r="AF152" s="3"/>
     </row>
-    <row r="153" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C153" s="1"/>
       <c r="D153" s="2"/>
       <c r="E153" s="2"/>
@@ -49467,7 +49473,7 @@
       <c r="AE153" s="3"/>
       <c r="AF153" s="3"/>
     </row>
-    <row r="154" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C154" s="1"/>
       <c r="D154" s="2"/>
       <c r="E154" s="2"/>
@@ -49499,7 +49505,7 @@
       <c r="AE154" s="3"/>
       <c r="AF154" s="3"/>
     </row>
-    <row r="155" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C155" s="1"/>
       <c r="D155" s="2"/>
       <c r="E155" s="2"/>
@@ -49531,7 +49537,7 @@
       <c r="AE155" s="3"/>
       <c r="AF155" s="3"/>
     </row>
-    <row r="156" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C156" s="1"/>
       <c r="D156" s="2"/>
       <c r="E156" s="2"/>
@@ -49563,7 +49569,7 @@
       <c r="AE156" s="3"/>
       <c r="AF156" s="3"/>
     </row>
-    <row r="157" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C157" s="1"/>
       <c r="D157" s="2"/>
       <c r="E157" s="2"/>
@@ -49595,7 +49601,7 @@
       <c r="AE157" s="3"/>
       <c r="AF157" s="3"/>
     </row>
-    <row r="158" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C158" s="1"/>
       <c r="D158" s="2"/>
       <c r="E158" s="2"/>
@@ -49627,7 +49633,7 @@
       <c r="AE158" s="3"/>
       <c r="AF158" s="3"/>
     </row>
-    <row r="159" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C159" s="1"/>
       <c r="D159" s="2"/>
       <c r="E159" s="2"/>
@@ -49659,7 +49665,7 @@
       <c r="AE159" s="3"/>
       <c r="AF159" s="3"/>
     </row>
-    <row r="160" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C160" s="1"/>
       <c r="D160" s="2"/>
       <c r="E160" s="2"/>
@@ -49691,7 +49697,7 @@
       <c r="AE160" s="3"/>
       <c r="AF160" s="3"/>
     </row>
-    <row r="161" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="161" spans="3:32" x14ac:dyDescent="0.2">
       <c r="C161" s="1"/>
       <c r="D161" s="2"/>
       <c r="E161" s="2"/>
@@ -49723,7 +49729,7 @@
       <c r="AE161" s="3"/>
       <c r="AF161" s="3"/>
     </row>
-    <row r="162" spans="3:32" ht="15" x14ac:dyDescent="0.2">
+    <row r="162" spans="3:32" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C162" s="1"/>
       <c r="D162" s="2"/>
       <c r="E162" s="2"/>
@@ -49755,7 +49761,7 @@
       <c r="AE162" s="3"/>
       <c r="AF162" s="3"/>
     </row>
-    <row r="163" spans="3:32" ht="15" x14ac:dyDescent="0.2">
+    <row r="163" spans="3:32" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C163" s="1"/>
       <c r="D163" s="2"/>
       <c r="E163" s="2"/>
@@ -49786,7 +49792,7 @@
       <c r="AE163" s="3"/>
       <c r="AF163" s="3"/>
     </row>
-    <row r="164" spans="3:32" ht="14" x14ac:dyDescent="0.15">
+    <row r="164" spans="3:32" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C164" s="1"/>
       <c r="D164" s="2"/>
       <c r="E164" s="2"/>
@@ -49814,7 +49820,7 @@
       <c r="AE164" s="3"/>
       <c r="AF164" s="43"/>
     </row>
-    <row r="165" spans="3:32" ht="15" x14ac:dyDescent="0.2">
+    <row r="165" spans="3:32" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C165" s="1"/>
       <c r="D165" s="2"/>
       <c r="E165" s="2"/>
@@ -49838,7 +49844,7 @@
       <c r="AE165" s="3"/>
       <c r="AF165" s="3"/>
     </row>
-    <row r="166" spans="3:32" ht="15" x14ac:dyDescent="0.2">
+    <row r="166" spans="3:32" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C166" s="1"/>
       <c r="D166" s="2"/>
       <c r="E166" s="2"/>
@@ -49857,7 +49863,7 @@
       <c r="R166" s="1"/>
       <c r="AE166" s="3"/>
     </row>
-    <row r="167" spans="3:32" ht="15" x14ac:dyDescent="0.2">
+    <row r="167" spans="3:32" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C167" s="1"/>
       <c r="D167" s="2"/>
       <c r="E167" s="2"/>
@@ -49876,7 +49882,7 @@
       <c r="R167" s="1"/>
       <c r="AE167" s="3"/>
     </row>
-    <row r="168" spans="3:32" ht="15" x14ac:dyDescent="0.2">
+    <row r="168" spans="3:32" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C168" s="1"/>
       <c r="D168" s="2"/>
       <c r="E168" s="2"/>
@@ -49895,7 +49901,7 @@
       <c r="R168" s="1"/>
       <c r="AE168" s="3"/>
     </row>
-    <row r="169" spans="3:32" ht="15" x14ac:dyDescent="0.2">
+    <row r="169" spans="3:32" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C169" s="1"/>
       <c r="D169" s="2"/>
       <c r="E169" s="2"/>
@@ -49914,7 +49920,7 @@
       <c r="R169" s="1"/>
       <c r="AE169" s="3"/>
     </row>
-    <row r="170" spans="3:32" ht="15" x14ac:dyDescent="0.2">
+    <row r="170" spans="3:32" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C170" s="1"/>
       <c r="D170" s="2"/>
       <c r="E170" s="2"/>
@@ -49933,7 +49939,7 @@
       <c r="R170" s="1"/>
       <c r="AE170" s="3"/>
     </row>
-    <row r="171" spans="3:32" ht="15" x14ac:dyDescent="0.2">
+    <row r="171" spans="3:32" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C171" s="1"/>
       <c r="D171" s="2"/>
       <c r="E171" s="2"/>
@@ -49952,7 +49958,7 @@
       <c r="R171" s="1"/>
       <c r="AE171" s="3"/>
     </row>
-    <row r="172" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="172" spans="3:32" x14ac:dyDescent="0.2">
       <c r="C172" s="1"/>
       <c r="D172" s="2"/>
       <c r="E172" s="2"/>
@@ -49975,7 +49981,7 @@
       <c r="V172" s="3"/>
       <c r="AE172" s="3"/>
     </row>
-    <row r="173" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="173" spans="3:32" x14ac:dyDescent="0.2">
       <c r="C173" s="1"/>
       <c r="D173" s="2"/>
       <c r="E173" s="2"/>
@@ -50007,7 +50013,7 @@
       <c r="AE173" s="3"/>
       <c r="AF173" s="3"/>
     </row>
-    <row r="174" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="174" spans="3:32" x14ac:dyDescent="0.2">
       <c r="C174" s="1"/>
       <c r="D174" s="2"/>
       <c r="E174" s="2"/>
@@ -50039,7 +50045,7 @@
       <c r="AE174" s="3"/>
       <c r="AF174" s="3"/>
     </row>
-    <row r="175" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="175" spans="3:32" x14ac:dyDescent="0.2">
       <c r="C175" s="1"/>
       <c r="D175" s="2"/>
       <c r="E175" s="2"/>
@@ -50071,7 +50077,7 @@
       <c r="AE175" s="3"/>
       <c r="AF175" s="3"/>
     </row>
-    <row r="176" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="176" spans="3:32" x14ac:dyDescent="0.2">
       <c r="C176" s="1"/>
       <c r="D176" s="2"/>
       <c r="E176" s="2"/>
@@ -50103,7 +50109,7 @@
       <c r="AE176" s="3"/>
       <c r="AF176" s="3"/>
     </row>
-    <row r="177" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="177" spans="3:32" x14ac:dyDescent="0.2">
       <c r="C177" s="1"/>
       <c r="D177" s="2"/>
       <c r="E177" s="2"/>
@@ -50135,7 +50141,7 @@
       <c r="AE177" s="3"/>
       <c r="AF177" s="3"/>
     </row>
-    <row r="178" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="178" spans="3:32" x14ac:dyDescent="0.2">
       <c r="C178" s="1"/>
       <c r="D178" s="2"/>
       <c r="E178" s="2"/>
@@ -50167,7 +50173,7 @@
       <c r="AE178" s="3"/>
       <c r="AF178" s="3"/>
     </row>
-    <row r="179" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="179" spans="3:32" x14ac:dyDescent="0.2">
       <c r="C179" s="1"/>
       <c r="D179" s="2"/>
       <c r="E179" s="2"/>
@@ -50199,7 +50205,7 @@
       <c r="AE179" s="3"/>
       <c r="AF179" s="3"/>
     </row>
-    <row r="180" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="180" spans="3:32" x14ac:dyDescent="0.2">
       <c r="C180" s="1"/>
       <c r="D180" s="2"/>
       <c r="E180" s="2"/>
@@ -50231,7 +50237,7 @@
       <c r="AE180" s="3"/>
       <c r="AF180" s="3"/>
     </row>
-    <row r="181" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="181" spans="3:32" x14ac:dyDescent="0.2">
       <c r="C181" s="1"/>
       <c r="D181" s="2"/>
       <c r="E181" s="2"/>
@@ -50263,7 +50269,7 @@
       <c r="AE181" s="3"/>
       <c r="AF181" s="3"/>
     </row>
-    <row r="182" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="182" spans="3:32" x14ac:dyDescent="0.2">
       <c r="C182" s="1"/>
       <c r="D182" s="2"/>
       <c r="E182" s="2"/>
@@ -50295,7 +50301,7 @@
       <c r="AE182" s="3"/>
       <c r="AF182" s="3"/>
     </row>
-    <row r="183" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="183" spans="3:32" x14ac:dyDescent="0.2">
       <c r="C183" s="1"/>
       <c r="D183" s="2"/>
       <c r="E183" s="2"/>
@@ -50327,7 +50333,7 @@
       <c r="AE183" s="3"/>
       <c r="AF183" s="3"/>
     </row>
-    <row r="184" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="184" spans="3:32" x14ac:dyDescent="0.2">
       <c r="D184" s="2"/>
       <c r="E184" s="2"/>
       <c r="F184" s="2"/>
@@ -50358,7 +50364,7 @@
       <c r="AE184" s="3"/>
       <c r="AF184" s="3"/>
     </row>
-    <row r="185" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="185" spans="3:32" x14ac:dyDescent="0.2">
       <c r="D185" s="2"/>
       <c r="E185" s="2"/>
       <c r="F185" s="2"/>
@@ -50389,7 +50395,7 @@
       <c r="AE185" s="3"/>
       <c r="AF185" s="3"/>
     </row>
-    <row r="186" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="186" spans="3:32" x14ac:dyDescent="0.2">
       <c r="D186" s="2"/>
       <c r="E186" s="2"/>
       <c r="F186" s="2"/>
@@ -50420,7 +50426,7 @@
       <c r="AE186" s="3"/>
       <c r="AF186" s="3"/>
     </row>
-    <row r="187" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="187" spans="3:32" x14ac:dyDescent="0.2">
       <c r="D187" s="2"/>
       <c r="E187" s="2"/>
       <c r="F187" s="2"/>
@@ -50451,7 +50457,7 @@
       <c r="AE187" s="3"/>
       <c r="AF187" s="3"/>
     </row>
-    <row r="188" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="188" spans="3:32" x14ac:dyDescent="0.2">
       <c r="D188" s="2"/>
       <c r="E188" s="2"/>
       <c r="F188" s="2"/>
@@ -50482,7 +50488,7 @@
       <c r="AE188" s="3"/>
       <c r="AF188" s="3"/>
     </row>
-    <row r="189" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="189" spans="3:32" x14ac:dyDescent="0.2">
       <c r="D189" s="2"/>
       <c r="E189" s="2"/>
       <c r="F189" s="2"/>
@@ -50513,7 +50519,7 @@
       <c r="AE189" s="3"/>
       <c r="AF189" s="3"/>
     </row>
-    <row r="190" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="190" spans="3:32" x14ac:dyDescent="0.2">
       <c r="D190" s="2"/>
       <c r="E190" s="2"/>
       <c r="F190" s="2"/>
@@ -50544,7 +50550,7 @@
       <c r="AE190" s="3"/>
       <c r="AF190" s="3"/>
     </row>
-    <row r="191" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="191" spans="3:32" x14ac:dyDescent="0.2">
       <c r="D191" s="2"/>
       <c r="E191" s="2"/>
       <c r="F191" s="2"/>
@@ -50575,7 +50581,7 @@
       <c r="AE191" s="3"/>
       <c r="AF191" s="3"/>
     </row>
-    <row r="192" spans="3:32" x14ac:dyDescent="0.15">
+    <row r="192" spans="3:32" x14ac:dyDescent="0.2">
       <c r="D192" s="2"/>
       <c r="E192" s="2"/>
       <c r="F192" s="2"/>
@@ -50606,7 +50612,7 @@
       <c r="AE192" s="3"/>
       <c r="AF192" s="3"/>
     </row>
-    <row r="193" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="193" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D193" s="2"/>
       <c r="E193" s="2"/>
       <c r="F193" s="2"/>
@@ -50637,7 +50643,7 @@
       <c r="AE193" s="3"/>
       <c r="AF193" s="3"/>
     </row>
-    <row r="194" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="194" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D194" s="2"/>
       <c r="E194" s="2"/>
       <c r="F194" s="2"/>
@@ -50668,7 +50674,7 @@
       <c r="AE194" s="3"/>
       <c r="AF194" s="3"/>
     </row>
-    <row r="195" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="195" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D195" s="2"/>
       <c r="E195" s="2"/>
       <c r="F195" s="2"/>
@@ -50699,7 +50705,7 @@
       <c r="AE195" s="3"/>
       <c r="AF195" s="3"/>
     </row>
-    <row r="196" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="196" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D196" s="2"/>
       <c r="E196" s="2"/>
       <c r="F196" s="2"/>
@@ -50730,7 +50736,7 @@
       <c r="AE196" s="3"/>
       <c r="AF196" s="3"/>
     </row>
-    <row r="197" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="197" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D197" s="2"/>
       <c r="E197" s="2"/>
       <c r="F197" s="2"/>
@@ -50761,7 +50767,7 @@
       <c r="AE197" s="3"/>
       <c r="AF197" s="3"/>
     </row>
-    <row r="198" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="198" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D198" s="2"/>
       <c r="E198" s="2"/>
       <c r="F198" s="2"/>
@@ -50792,7 +50798,7 @@
       <c r="AE198" s="3"/>
       <c r="AF198" s="3"/>
     </row>
-    <row r="199" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="199" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D199" s="2"/>
       <c r="E199" s="2"/>
       <c r="F199" s="2"/>
@@ -50823,7 +50829,7 @@
       <c r="AE199" s="3"/>
       <c r="AF199" s="3"/>
     </row>
-    <row r="200" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="200" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D200" s="2"/>
       <c r="E200" s="2"/>
       <c r="F200" s="2"/>
@@ -50854,7 +50860,7 @@
       <c r="AE200" s="3"/>
       <c r="AF200" s="3"/>
     </row>
-    <row r="201" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="201" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D201" s="2"/>
       <c r="E201" s="2"/>
       <c r="F201" s="2"/>
@@ -50885,7 +50891,7 @@
       <c r="AE201" s="3"/>
       <c r="AF201" s="3"/>
     </row>
-    <row r="202" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="202" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D202" s="2"/>
       <c r="E202" s="2"/>
       <c r="F202" s="2"/>
@@ -50916,7 +50922,7 @@
       <c r="AE202" s="3"/>
       <c r="AF202" s="3"/>
     </row>
-    <row r="203" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="203" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D203" s="2"/>
       <c r="E203" s="2"/>
       <c r="F203" s="2"/>
@@ -50947,7 +50953,7 @@
       <c r="AE203" s="3"/>
       <c r="AF203" s="3"/>
     </row>
-    <row r="204" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="204" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D204" s="2"/>
       <c r="E204" s="2"/>
       <c r="F204" s="2"/>
@@ -50978,7 +50984,7 @@
       <c r="AE204" s="3"/>
       <c r="AF204" s="3"/>
     </row>
-    <row r="205" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="205" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D205" s="2"/>
       <c r="E205" s="2"/>
       <c r="F205" s="2"/>
@@ -51009,7 +51015,7 @@
       <c r="AE205" s="3"/>
       <c r="AF205" s="3"/>
     </row>
-    <row r="206" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="206" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D206" s="2"/>
       <c r="E206" s="2"/>
       <c r="F206" s="2"/>
@@ -51040,7 +51046,7 @@
       <c r="AE206" s="3"/>
       <c r="AF206" s="3"/>
     </row>
-    <row r="207" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="207" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D207" s="2"/>
       <c r="E207" s="2"/>
       <c r="F207" s="2"/>
@@ -51071,7 +51077,7 @@
       <c r="AE207" s="3"/>
       <c r="AF207" s="3"/>
     </row>
-    <row r="208" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="208" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D208" s="2"/>
       <c r="E208" s="2"/>
       <c r="F208" s="2"/>
@@ -51102,7 +51108,7 @@
       <c r="AE208" s="3"/>
       <c r="AF208" s="3"/>
     </row>
-    <row r="209" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="209" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D209" s="2"/>
       <c r="E209" s="2"/>
       <c r="F209" s="2"/>
@@ -51133,7 +51139,7 @@
       <c r="AE209" s="3"/>
       <c r="AF209" s="3"/>
     </row>
-    <row r="210" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="210" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D210" s="2"/>
       <c r="E210" s="2"/>
       <c r="F210" s="2"/>
@@ -51164,7 +51170,7 @@
       <c r="AE210" s="3"/>
       <c r="AF210" s="3"/>
     </row>
-    <row r="211" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="211" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D211" s="2"/>
       <c r="E211" s="2"/>
       <c r="F211" s="2"/>
@@ -51195,7 +51201,7 @@
       <c r="AE211" s="3"/>
       <c r="AF211" s="3"/>
     </row>
-    <row r="212" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="212" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D212" s="2"/>
       <c r="E212" s="2"/>
       <c r="F212" s="2"/>
@@ -51226,7 +51232,7 @@
       <c r="AE212" s="3"/>
       <c r="AF212" s="3"/>
     </row>
-    <row r="213" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="213" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D213" s="2"/>
       <c r="E213" s="2"/>
       <c r="F213" s="2"/>
@@ -51257,7 +51263,7 @@
       <c r="AE213" s="3"/>
       <c r="AF213" s="3"/>
     </row>
-    <row r="214" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="214" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D214" s="2"/>
       <c r="E214" s="2"/>
       <c r="F214" s="2"/>
@@ -51288,7 +51294,7 @@
       <c r="AE214" s="3"/>
       <c r="AF214" s="3"/>
     </row>
-    <row r="215" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="215" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D215" s="2"/>
       <c r="E215" s="2"/>
       <c r="F215" s="2"/>
@@ -51319,7 +51325,7 @@
       <c r="AE215" s="3"/>
       <c r="AF215" s="3"/>
     </row>
-    <row r="216" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="216" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D216" s="2"/>
       <c r="E216" s="2"/>
       <c r="F216" s="2"/>
@@ -51350,7 +51356,7 @@
       <c r="AE216" s="3"/>
       <c r="AF216" s="3"/>
     </row>
-    <row r="217" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="217" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D217" s="2"/>
       <c r="E217" s="2"/>
       <c r="F217" s="2"/>
@@ -51381,7 +51387,7 @@
       <c r="AE217" s="3"/>
       <c r="AF217" s="3"/>
     </row>
-    <row r="218" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="218" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D218" s="2"/>
       <c r="E218" s="2"/>
       <c r="F218" s="2"/>
@@ -51412,7 +51418,7 @@
       <c r="AE218" s="3"/>
       <c r="AF218" s="3"/>
     </row>
-    <row r="219" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="219" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D219" s="2"/>
       <c r="E219" s="2"/>
       <c r="F219" s="2"/>
@@ -51443,7 +51449,7 @@
       <c r="AE219" s="3"/>
       <c r="AF219" s="3"/>
     </row>
-    <row r="220" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="220" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D220" s="2"/>
       <c r="E220" s="2"/>
       <c r="F220" s="2"/>
@@ -51474,7 +51480,7 @@
       <c r="AE220" s="3"/>
       <c r="AF220" s="3"/>
     </row>
-    <row r="221" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="221" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D221" s="2"/>
       <c r="E221" s="2"/>
       <c r="F221" s="2"/>
@@ -51505,7 +51511,7 @@
       <c r="AE221" s="3"/>
       <c r="AF221" s="3"/>
     </row>
-    <row r="222" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="222" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D222" s="2"/>
       <c r="E222" s="2"/>
       <c r="F222" s="2"/>
@@ -51536,7 +51542,7 @@
       <c r="AE222" s="3"/>
       <c r="AF222" s="3"/>
     </row>
-    <row r="223" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="223" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D223" s="2"/>
       <c r="E223" s="2"/>
       <c r="F223" s="2"/>
@@ -51567,7 +51573,7 @@
       <c r="AE223" s="3"/>
       <c r="AF223" s="3"/>
     </row>
-    <row r="224" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="224" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D224" s="2"/>
       <c r="E224" s="2"/>
       <c r="F224" s="2"/>
@@ -51598,7 +51604,7 @@
       <c r="AE224" s="3"/>
       <c r="AF224" s="3"/>
     </row>
-    <row r="225" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="225" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D225" s="2"/>
       <c r="E225" s="2"/>
       <c r="F225" s="2"/>
@@ -51629,7 +51635,7 @@
       <c r="AE225" s="3"/>
       <c r="AF225" s="3"/>
     </row>
-    <row r="226" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="226" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D226" s="2"/>
       <c r="E226" s="2"/>
       <c r="F226" s="2"/>
@@ -51660,7 +51666,7 @@
       <c r="AE226" s="3"/>
       <c r="AF226" s="3"/>
     </row>
-    <row r="227" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="227" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D227" s="2"/>
       <c r="E227" s="2"/>
       <c r="F227" s="2"/>
@@ -51691,7 +51697,7 @@
       <c r="AE227" s="3"/>
       <c r="AF227" s="3"/>
     </row>
-    <row r="228" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="228" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D228" s="2"/>
       <c r="E228" s="2"/>
       <c r="F228" s="2"/>
@@ -51722,7 +51728,7 @@
       <c r="AE228" s="3"/>
       <c r="AF228" s="3"/>
     </row>
-    <row r="229" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="229" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D229" s="2"/>
       <c r="E229" s="2"/>
       <c r="F229" s="2"/>
@@ -51753,7 +51759,7 @@
       <c r="AE229" s="3"/>
       <c r="AF229" s="3"/>
     </row>
-    <row r="230" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="230" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D230" s="2"/>
       <c r="E230" s="2"/>
       <c r="F230" s="2"/>
@@ -51784,7 +51790,7 @@
       <c r="AE230" s="3"/>
       <c r="AF230" s="3"/>
     </row>
-    <row r="231" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="231" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D231" s="2"/>
       <c r="E231" s="2"/>
       <c r="F231" s="2"/>
@@ -51815,7 +51821,7 @@
       <c r="AE231" s="3"/>
       <c r="AF231" s="3"/>
     </row>
-    <row r="232" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="232" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D232" s="2"/>
       <c r="E232" s="2"/>
       <c r="F232" s="2"/>
@@ -51846,7 +51852,7 @@
       <c r="AE232" s="3"/>
       <c r="AF232" s="3"/>
     </row>
-    <row r="233" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="233" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D233" s="2"/>
       <c r="E233" s="2"/>
       <c r="F233" s="2"/>
@@ -51877,7 +51883,7 @@
       <c r="AE233" s="3"/>
       <c r="AF233" s="3"/>
     </row>
-    <row r="234" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="234" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D234" s="2"/>
       <c r="E234" s="2"/>
       <c r="F234" s="2"/>
@@ -51908,7 +51914,7 @@
       <c r="AE234" s="3"/>
       <c r="AF234" s="3"/>
     </row>
-    <row r="235" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="235" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D235" s="2"/>
       <c r="E235" s="2"/>
       <c r="F235" s="2"/>
@@ -51939,7 +51945,7 @@
       <c r="AE235" s="3"/>
       <c r="AF235" s="3"/>
     </row>
-    <row r="236" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="236" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D236" s="2"/>
       <c r="E236" s="2"/>
       <c r="F236" s="2"/>
@@ -51972,7 +51978,7 @@
       <c r="AE236" s="3"/>
       <c r="AF236" s="3"/>
     </row>
-    <row r="237" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="237" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D237" s="2"/>
       <c r="E237" s="2"/>
       <c r="F237" s="2"/>
@@ -52003,7 +52009,7 @@
       <c r="AE237" s="3"/>
       <c r="AF237" s="3"/>
     </row>
-    <row r="238" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="238" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D238" s="2"/>
       <c r="E238" s="2"/>
       <c r="F238" s="2"/>
@@ -52034,7 +52040,7 @@
       <c r="AE238" s="3"/>
       <c r="AF238" s="3"/>
     </row>
-    <row r="239" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="239" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D239" s="2"/>
       <c r="E239" s="2"/>
       <c r="F239" s="2"/>
@@ -52065,7 +52071,7 @@
       <c r="AE239" s="3"/>
       <c r="AF239" s="3"/>
     </row>
-    <row r="240" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="240" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D240" s="2"/>
       <c r="E240" s="2"/>
       <c r="F240" s="2"/>
@@ -52096,7 +52102,7 @@
       <c r="AE240" s="3"/>
       <c r="AF240" s="3"/>
     </row>
-    <row r="241" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="241" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D241" s="2"/>
       <c r="E241" s="2"/>
       <c r="F241" s="2"/>
@@ -52127,7 +52133,7 @@
       <c r="AE241" s="3"/>
       <c r="AF241" s="3"/>
     </row>
-    <row r="242" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="242" spans="4:32" x14ac:dyDescent="0.2">
       <c r="P242" s="1"/>
       <c r="Q242" s="3"/>
       <c r="R242" s="3"/>
@@ -52146,7 +52152,7 @@
       <c r="AE242" s="3"/>
       <c r="AF242" s="3"/>
     </row>
-    <row r="243" spans="4:32" x14ac:dyDescent="0.15">
+    <row r="243" spans="4:32" x14ac:dyDescent="0.2">
       <c r="W243" s="2"/>
       <c r="X243" s="3"/>
       <c r="Y243" s="3"/>
@@ -52165,7 +52171,7 @@
     <protectedRange sqref="P53:Q67 P69:Q83 P85:Q99 P101:Q115 P117:Q131 P133:Q147 P21:Q35 P37:Q51" name="Gln_Glu_2"/>
     <protectedRange sqref="N21:O37 N117:O133 N85:O101 N53:N69 O54:O69" name="cell number_all_1"/>
     <protectedRange sqref="Y67 Y53:Y65 Y69:Y71 Y101:Y103 Y133:Y135 Y21:Y38 Y85:Y99 Y117:Y131" name="sample_vol_base_1"/>
-    <protectedRange sqref="S53:U59 S117:U123 S85:U91 AA53:AA59 S21:U27 AA69:AA74 AA85:AA91 AA101:AA106 AC133:AC135 AA117:AA123 AA133:AA136 AA21:AA27 AC53:AC59 AC69:AC74 AC85:AC91 AC101:AC106 AC117:AC123 AC21:AC27 X53:X67 X69:X83 X85:X99 X101:X115 X117:X131 X133:X147 X21:X35 X37:X51 Z20:Z147 AB20:AB147 AD20:AD147" name="osmolality_1"/>
+    <protectedRange sqref="S53:U59 S117:U123 S85:U91 AA53:AA59 S21:U27 AA69:AA74 AA85:AA91 AA101:AA106 AC133:AC135 AA117:AA123 AA133:AA136 AA21:AA27 AC53:AC59 AC69:AC74 AC85:AC91 AC101:AC106 AC117:AC123 AC21:AC27 X53:X67 X69:X83 X85:X99 X101:X115 X117:X131 X133:X147 X21:X35 X37:X51 AB20:AB147 AD20:AD147 Z20:Z147" name="osmolality_1"/>
     <protectedRange sqref="Y67 Y53:Y65 Y69:Y71 Y101:Y103 Y133:Y135 Y21:Y38 Y85:Y99 Y117:Y131" name="total_volume"/>
     <protectedRange sqref="Y67 Y53:Y65 Y69:Y71 Y101:Y103 Y133:Y135 Y21:Y38 Y85:Y99 Y117:Y131" name="protein_total_yield_NH3"/>
     <protectedRange sqref="S134:U147 S70:U83 S38:U51 S102:U115 AC38:AC51 AA75:AA83 AA107:AA115 AA137:AA147 AC75:AC83 AC107:AC115 AA38:AA51 AC136:AC147" name="osmolality_2"/>
@@ -52186,9 +52192,10 @@
     <protectedRange sqref="V21:V35 V94:V99 V62:V67 V53:V60 V110:V111 V126:V131 V142:V143 V37:V44 V69:V76 V85:V89 V101:V105 V117:V121 V133:V137" name="Glc_Lac_1_1"/>
     <protectedRange sqref="V61 V90:V93 V77:V83 V144:V147 V112:V115 V45:V51 V106:V109 V122:V125 V138:V141" name="sample_vol_base_2_1"/>
   </protectedRanges>
+  <phoneticPr fontId="35" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>